<commit_message>
update the test files
Change-Id: I0285e9d6739e7f2a9882fd19f03524482128e2d2
</commit_message>
<xml_diff>
--- a/sc/qa/unit/data/xlsx/databar.xlsx
+++ b/sc/qa/unit/data/xlsx/databar.xlsx
@@ -108,7 +108,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E15" activeCellId="0" pane="topLeft" sqref="E15"/>
+      <selection activeCell="I4" activeCellId="0" pane="topLeft" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -207,7 +207,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{30778D12-BFAB-40E5-8C37-AACABF616153}</x14:id>
+          <x14:id>{EE42C722-2BA3-45CF-8C3D-502D41881B21}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -221,7 +221,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{AD18CFCB-7363-4813-A1AF-75A36CEFADD9}</x14:id>
+          <x14:id>{5490D118-20FB-4947-B2E6-B8787AA14197}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -235,27 +235,13 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7F5AF51A-3BE6-4722-A13E-2B285AF13BE7}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H6">
+          <x14:id>{56789476-A957-4E9A-BB9C-8B9A82703C59}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:B13">
     <cfRule priority="5" type="dataBar">
-      <dataBar>
-        <cfvo type="num" val="-2"/>
-        <cfvo type="formula" val=""/>
-        <color rgb="FF0000FF"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{28E96DFC-B046-499A-A65E-B6D0901F7463}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B10:B13">
-    <cfRule priority="6" type="dataBar">
       <dataBar>
         <cfvo type="min" val="0"/>
         <cfvo type="max" val="0"/>
@@ -263,7 +249,21 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{30E139BC-6CB6-4089-AA62-F466E647ED81}</x14:id>
+          <x14:id>{D011C2F0-3F76-46ED-BB39-B9D96B695D31}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H6">
+    <cfRule priority="6" type="dataBar">
+      <dataBar>
+        <cfvo type="num" val="-2"/>
+        <cfvo type="formula" val="3*A1+2"/>
+        <color rgb="FF0000FF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{B4849452-58A6-4E59-BC92-582BFA343E11}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -279,7 +279,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule id="{30778D12-BFAB-40E5-8C37-AACABF616153}" type="dataBar">
+          <x14:cfRule id="{EE42C722-2BA3-45CF-8C3D-502D41881B21}" type="dataBar">
             <x14:dataBar axisPosition="automatic" maxLength="100" minLength="0">
               <x14:cfvo type="autoMin" value="0"/>
               <x14:cfvo type="autoMax" value="0"/>
@@ -290,7 +290,7 @@
           <xm:sqref>B3:B6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule id="{AD18CFCB-7363-4813-A1AF-75A36CEFADD9}" type="dataBar">
+          <x14:cfRule id="{5490D118-20FB-4947-B2E6-B8787AA14197}" type="dataBar">
             <x14:dataBar axisPosition="automatic" maxLength="100" minLength="0">
               <x14:cfvo type="min" value="0"/>
               <x14:cfvo type="max" value="0"/>
@@ -301,7 +301,7 @@
           <xm:sqref>D3:D6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule id="{7F5AF51A-3BE6-4722-A13E-2B285AF13BE7}" type="dataBar">
+          <x14:cfRule id="{56789476-A957-4E9A-BB9C-8B9A82703C59}" type="dataBar">
             <x14:dataBar axisPosition="automatic" maxLength="100" minLength="0">
               <x14:cfvo type="percentile" value="10"/>
               <x14:cfvo type="percent" value="90"/>
@@ -312,18 +312,7 @@
           <xm:sqref>F3:F6</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule id="{28E96DFC-B046-499A-A65E-B6D0901F7463}" type="dataBar">
-            <x14:dataBar axisPosition="automatic" maxLength="100" minLength="0">
-              <x14:cfvo type="num" value="-2"/>
-              <x14:cfvo type="formula" value=""/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>H3:H6</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule id="{30E139BC-6CB6-4089-AA62-F466E647ED81}" type="dataBar">
+          <x14:cfRule id="{D011C2F0-3F76-46ED-BB39-B9D96B695D31}" type="dataBar">
             <x14:dataBar axisPosition="middle" maxLength="100" minLength="0">
               <x14:cfvo type="autoMin" value="0"/>
               <x14:cfvo type="autoMax" value="0"/>
@@ -333,6 +322,17 @@
           </x14:cfRule>
           <xm:sqref>B10:B13</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule id="{B4849452-58A6-4E59-BC92-582BFA343E11}" type="dataBar">
+            <x14:dataBar axisPosition="automatic" maxLength="100" minLength="0">
+              <x14:cfvo type="num" value="-2"/>
+              <x14:cfvo type="formula" value="3*A1+2"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H3:H6</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>